<commit_message>
fixes to gradient calculation, added testing code
</commit_message>
<xml_diff>
--- a/parameter_files/de_dg_gw_lower.xlsx
+++ b/parameter_files/de_dg_gw_lower.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4efc3e9dc81381f4/Documents/SJV-gen-modeling/parameter_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="8_{229B6D89-0FBA-4AFF-BE65-AE5ED1F338BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06191D24-75D4-43FD-B9AD-064788079556}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="8_{229B6D89-0FBA-4AFF-BE65-AE5ED1F338BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F31B66AC-630F-4CAD-A4F1-B408AAF68056}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{47BB98F9-56B8-471D-9F66-573A44E98337}"/>
   </bookViews>
@@ -35,24 +35,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
-    <t>small growers to gw</t>
-  </si>
-  <si>
-    <t>large growers to gw</t>
-  </si>
-  <si>
-    <t>small growers (white area) to gw</t>
-  </si>
-  <si>
-    <t>large growers (white area) to gw</t>
-  </si>
-  <si>
-    <t>rural communities to gw</t>
-  </si>
-  <si>
-    <t>municipalities to gw</t>
-  </si>
-  <si>
     <t>Bureau of Reclamation</t>
   </si>
   <si>
@@ -138,13 +120,31 @@
   </si>
   <si>
     <t>environmental orgs</t>
+  </si>
+  <si>
+    <t>rural communities</t>
+  </si>
+  <si>
+    <t>small growers</t>
+  </si>
+  <si>
+    <t>investor growers</t>
+  </si>
+  <si>
+    <t>small growers (white area)</t>
+  </si>
+  <si>
+    <t>investor growers (white area)</t>
+  </si>
+  <si>
+    <t>municipalities</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,6 +177,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -186,7 +192,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -259,7 +265,7 @@
         <color rgb="FFCCCCCC"/>
       </left>
       <right style="medium">
-        <color rgb="FFCCCCCC"/>
+        <color rgb="FF000000"/>
       </right>
       <top/>
       <bottom/>
@@ -269,18 +275,35 @@
       <left style="medium">
         <color rgb="FFCCCCCC"/>
       </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
+      <right style="thin">
+        <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -303,11 +326,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -630,41 +656,42 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomRight" activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="28.7265625" customWidth="1"/>
+    <col min="2" max="2" width="13.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="64" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="8" t="s">
         <v>29</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -675,7 +702,7 @@
     </row>
     <row r="3" spans="1:8" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="7" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -686,7 +713,7 @@
     </row>
     <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="7" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -697,7 +724,7 @@
     </row>
     <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="7" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -708,7 +735,7 @@
     </row>
     <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="7" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -719,7 +746,7 @@
     </row>
     <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="7" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B7" s="4">
         <v>0</v>
@@ -732,7 +759,7 @@
     </row>
     <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -743,7 +770,7 @@
     </row>
     <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="7" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -753,13 +780,13 @@
       <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="10" t="s">
-        <v>34</v>
+      <c r="A10" s="9" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -770,7 +797,7 @@
     </row>
     <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -781,7 +808,7 @@
     </row>
     <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="3" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -792,7 +819,7 @@
     </row>
     <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -803,7 +830,7 @@
     </row>
     <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -814,7 +841,7 @@
     </row>
     <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -824,8 +851,8 @@
       <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="9" t="s">
-        <v>30</v>
+      <c r="A17" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -835,8 +862,8 @@
       <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="9" t="s">
-        <v>31</v>
+      <c r="A18" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -846,8 +873,8 @@
       <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="9" t="s">
-        <v>32</v>
+      <c r="A19" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="B19" s="4">
         <v>0.5</v>
@@ -859,8 +886,8 @@
       <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="9" t="s">
-        <v>33</v>
+      <c r="A20" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="4"/>
@@ -871,7 +898,7 @@
     </row>
     <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="5"/>
@@ -882,7 +909,7 @@
     </row>
     <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B22" s="5">
         <v>0</v>
@@ -895,7 +922,7 @@
     </row>
     <row r="23" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B23" s="5">
         <v>0.5</v>
@@ -908,7 +935,7 @@
     </row>
     <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -919,7 +946,7 @@
     </row>
     <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -930,7 +957,7 @@
     </row>
     <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -941,7 +968,7 @@
     </row>
     <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -952,7 +979,7 @@
     </row>
     <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="6" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -963,7 +990,7 @@
     </row>
     <row r="29" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>

</xml_diff>